<commit_message>
finished the back end for the gems
</commit_message>
<xml_diff>
--- a/dndloot.xlsx
+++ b/dndloot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slimon/PycharmProjects/pythonProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E316F02C-F555-4E4A-A092-D4EC001B05A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8422F6F5-24AD-D14F-BB56-CCF3D72FF641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="2" r:id="rId1"/>
@@ -149,7 +149,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -158,12 +158,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-3d6 (10)</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>3d6 (10)</t>
         </r>
       </text>
     </comment>
@@ -173,7 +182,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -182,12 +191,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1d6 (3)</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1d6 (3)</t>
         </r>
       </text>
     </comment>
@@ -254,7 +272,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -263,12 +281,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-6d6 x 10 (210)</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>6d6 x 10 (210)</t>
         </r>
       </text>
     </comment>
@@ -303,7 +330,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -312,12 +339,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-3d6 x 10 (105)</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>3d6 x 10 (105)</t>
         </r>
       </text>
     </comment>
@@ -622,7 +658,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -631,12 +667,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-2d6 x 100 (700)</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2d6 x 100 (700)</t>
         </r>
       </text>
     </comment>
@@ -670,7 +715,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -679,12 +724,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-2d6 x 1,000 (7,000)</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2d6 x 1,000 (7,000)</t>
         </r>
       </text>
     </comment>
@@ -718,7 +772,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -727,12 +781,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1d6 x 1,000 (3,500)</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1d6 x 1,000 (3,500)</t>
         </r>
       </text>
     </comment>
@@ -790,7 +853,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -799,12 +862,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-2d6 x 100 (700)</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2d6 x 100 (700)</t>
         </r>
       </text>
     </comment>
@@ -846,7 +918,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -868,7 +940,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="671">
   <si>
     <t>Item Name</t>
   </si>
@@ -2878,6 +2950,9 @@
   </si>
   <si>
     <t>Rolled d10</t>
+  </si>
+  <si>
+    <t>GP worth</t>
   </si>
 </sst>
 </file>
@@ -3377,7 +3452,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3512,24 +3587,27 @@
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3550,19 +3628,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3577,6 +3652,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3597,7 +3673,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3885,7 +3961,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3897,7 +3973,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3913,8 +3989,8 @@
   </sheetPr>
   <dimension ref="A1:D344"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A273" workbookViewId="0">
+      <selection activeCell="A293" sqref="A293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8428,8 +8504,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="223" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8456,11 +8532,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>366</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
     </row>
     <row r="2" spans="1:21" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -8470,24 +8546,24 @@
         <v>368</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="61" t="s">
         <v>428</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="N2" s="61" t="s">
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="N2" s="62" t="s">
         <v>440</v>
       </c>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
@@ -8495,14 +8571,14 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
-      <c r="G3" s="63" t="s">
+      <c r="G3" s="75" t="s">
         <v>555</v>
       </c>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
       <c r="N3" s="3" t="s">
         <v>668</v>
       </c>
@@ -8554,9 +8630,10 @@
       <c r="L4" s="4" t="s">
         <v>439</v>
       </c>
+      <c r="M4" s="8"/>
       <c r="N4" s="8" cm="1">
         <f t="array" aca="1" ref="N4:N15" ca="1">_xlfn.RANDARRAY(12,1,1,12,TRUE)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O4" s="14">
         <v>1</v>
@@ -8605,9 +8682,9 @@
       <c r="L5" s="60">
         <v>1E-3</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="4">
         <f ca="1"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="O5" s="14">
         <v>2</v>
@@ -8656,9 +8733,9 @@
       <c r="L6" s="60">
         <v>0.01</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="4">
         <f ca="1"/>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="O6" s="14">
         <v>3</v>
@@ -8707,9 +8784,9 @@
       <c r="L7" s="60">
         <v>0.05</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="4">
         <f ca="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O7" s="14">
         <v>4</v>
@@ -8758,9 +8835,9 @@
       <c r="L8" s="60">
         <v>0.1</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="4">
         <f ca="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="O8" s="14">
         <v>5</v>
@@ -8809,7 +8886,7 @@
       <c r="L9" s="60">
         <v>1</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="4">
         <f ca="1"/>
         <v>5</v>
       </c>
@@ -8842,9 +8919,9 @@
       <c r="B10" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="4">
         <f ca="1"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="O10" s="14">
         <v>7</v>
@@ -8875,17 +8952,17 @@
       <c r="B11" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="G11" s="64" t="s">
+      <c r="G11" s="76" t="s">
         <v>556</v>
       </c>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="66"/>
-      <c r="N11" s="8">
+      <c r="H11" s="77"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="78"/>
+      <c r="N11" s="4">
         <f ca="1"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="O11" s="14">
         <v>8</v>
@@ -8934,9 +9011,9 @@
       <c r="L12" s="28" t="s">
         <v>562</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="4">
         <f ca="1"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="O12" s="14">
         <v>9</v>
@@ -8979,7 +9056,7 @@
       </c>
       <c r="H13" s="42">
         <f ca="1">Dice!C40</f>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="I13" s="43" t="s">
         <v>414</v>
@@ -8993,9 +9070,9 @@
       <c r="L13" s="44" t="s">
         <v>414</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="4">
         <f ca="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O13" s="14">
         <v>10</v>
@@ -9038,7 +9115,7 @@
       </c>
       <c r="I14" s="46">
         <f ca="1">Dice!C39</f>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J14" s="45" t="s">
         <v>414</v>
@@ -9049,9 +9126,9 @@
       <c r="L14" s="47" t="s">
         <v>414</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N14" s="4">
         <f ca="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O14" s="14">
         <v>11</v>
@@ -9100,7 +9177,7 @@
       </c>
       <c r="J15" s="46">
         <f ca="1">Dice!C38</f>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K15" s="45" t="s">
         <v>414</v>
@@ -9108,7 +9185,7 @@
       <c r="L15" s="47" t="s">
         <v>414</v>
       </c>
-      <c r="N15" s="8">
+      <c r="N15" s="4">
         <f ca="1"/>
         <v>6</v>
       </c>
@@ -9162,7 +9239,7 @@
       </c>
       <c r="K16" s="46">
         <f ca="1">Dice!C38</f>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="L16" s="47" t="s">
         <v>414</v>
@@ -9215,15 +9292,15 @@
       <c r="J18" s="50"/>
       <c r="K18" s="50"/>
       <c r="L18" s="51"/>
-      <c r="N18" s="62" t="s">
+      <c r="N18" s="61" t="s">
         <v>500</v>
       </c>
-      <c r="O18" s="62"/>
-      <c r="P18" s="62"/>
-      <c r="Q18" s="62"/>
-      <c r="R18" s="62"/>
-      <c r="S18" s="62"/>
-      <c r="T18" s="62"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="61"/>
       <c r="U18" s="2"/>
     </row>
     <row r="19" spans="1:21" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -9290,7 +9367,7 @@
       </c>
       <c r="H20" s="42">
         <f ca="1">Dice!C39*100</f>
-        <v>2000</v>
+        <v>1600</v>
       </c>
       <c r="I20" s="43" t="s">
         <v>414</v>
@@ -9307,7 +9384,7 @@
       </c>
       <c r="N20" s="8" cm="1">
         <f t="array" aca="1" ref="N20:N29" ca="1">_xlfn.RANDARRAY(10,1,1,10, TRUE)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="O20" s="8">
         <v>1</v>
@@ -9350,21 +9427,21 @@
       </c>
       <c r="I21" s="46">
         <f ca="1">Dice!C41*10</f>
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="J21" s="45" t="s">
         <v>414</v>
       </c>
-      <c r="K21" s="46">
-        <f ca="1">Dice!C37*10</f>
-        <v>110</v>
+      <c r="K21" s="46" t="e">
+        <f>Dice!#REF!*10</f>
+        <v>#REF!</v>
       </c>
       <c r="L21" s="47" t="s">
         <v>414</v>
       </c>
       <c r="N21" s="8">
         <f ca="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O21" s="8">
         <v>2</v>
@@ -9410,18 +9487,18 @@
       </c>
       <c r="J22" s="46">
         <f ca="1">Dice!C38*10</f>
-        <v>170</v>
-      </c>
-      <c r="K22" s="46">
-        <f ca="1">Dice!C37*10</f>
-        <v>110</v>
+        <v>140</v>
+      </c>
+      <c r="K22" s="46" t="e">
+        <f>Dice!#REF!*10</f>
+        <v>#REF!</v>
       </c>
       <c r="L22" s="47" t="s">
         <v>414</v>
       </c>
       <c r="N22" s="8">
         <f ca="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O22" s="8">
         <v>3</v>
@@ -9470,14 +9547,14 @@
       </c>
       <c r="K23" s="46">
         <f ca="1">Dice!C39*10</f>
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="L23" s="47" t="s">
         <v>414</v>
       </c>
       <c r="N23" s="8">
         <f ca="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O23" s="8">
         <v>4</v>
@@ -9524,17 +9601,17 @@
       <c r="J24" s="45" t="s">
         <v>414</v>
       </c>
-      <c r="K24" s="46">
-        <f ca="1">Dice!C37*10</f>
-        <v>110</v>
+      <c r="K24" s="46" t="e">
+        <f>Dice!#REF!*10</f>
+        <v>#REF!</v>
       </c>
       <c r="L24" s="48">
         <f ca="1">Dice!C38</f>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="N24" s="8">
         <f ca="1"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="O24" s="8">
         <v>5</v>
@@ -9570,7 +9647,7 @@
       <c r="L25" s="51"/>
       <c r="N25" s="8">
         <f ca="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O25" s="8">
         <v>6</v>
@@ -9661,7 +9738,7 @@
       </c>
       <c r="I27" s="42">
         <f ca="1">Dice!C39*100</f>
-        <v>2000</v>
+        <v>1600</v>
       </c>
       <c r="J27" s="43" t="s">
         <v>414</v>
@@ -9675,7 +9752,7 @@
       </c>
       <c r="N27" s="8">
         <f ca="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O27" s="8">
         <v>8</v>
@@ -9732,7 +9809,7 @@
       </c>
       <c r="N28" s="8">
         <f ca="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O28" s="8">
         <v>9</v>
@@ -9779,9 +9856,9 @@
       <c r="J29" s="45" t="s">
         <v>414</v>
       </c>
-      <c r="K29" s="46">
-        <f ca="1">Dice!C37*100</f>
-        <v>1100</v>
+      <c r="K29" s="46" t="e">
+        <f>Dice!#REF!*100</f>
+        <v>#REF!</v>
       </c>
       <c r="L29" s="48">
         <f ca="1">Dice!C36*10</f>
@@ -9789,7 +9866,7 @@
       </c>
       <c r="N29" s="8">
         <f ca="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O29" s="8">
         <v>10</v>
@@ -9836,13 +9913,13 @@
       <c r="J30" s="45" t="s">
         <v>414</v>
       </c>
-      <c r="K30" s="46">
-        <f ca="1">Dice!C37*100</f>
-        <v>1100</v>
-      </c>
-      <c r="L30" s="48">
-        <f ca="1">Dice!C37*10</f>
-        <v>110</v>
+      <c r="K30" s="46" t="e">
+        <f>Dice!#REF!*100</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L30" s="48" t="e">
+        <f>Dice!#REF!*10</f>
+        <v>#REF!</v>
       </c>
       <c r="O30" s="8"/>
     </row>
@@ -9910,13 +9987,13 @@
       <c r="I33" s="43" t="s">
         <v>414</v>
       </c>
-      <c r="J33" s="42">
-        <f ca="1">Dice!C37*1000</f>
-        <v>11000</v>
+      <c r="J33" s="42" t="e">
+        <f>Dice!#REF!*1000</f>
+        <v>#REF!</v>
       </c>
       <c r="K33" s="42">
         <f ca="1">Dice!C43*100</f>
-        <v>3500</v>
+        <v>3200</v>
       </c>
       <c r="L33" s="44" t="s">
         <v>414</v>
@@ -9989,9 +10066,9 @@
         <f ca="1">Dice!C36*1000</f>
         <v>5000</v>
       </c>
-      <c r="L35" s="54">
-        <f ca="1">Dice!C37*10</f>
-        <v>110</v>
+      <c r="L35" s="54" t="e">
+        <f>Dice!#REF!*10</f>
+        <v>#REF!</v>
       </c>
       <c r="O35" s="8"/>
     </row>
@@ -10009,14 +10086,14 @@
       <c r="A37" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="G37" s="68" t="s">
+      <c r="G37" s="69" t="s">
         <v>663</v>
       </c>
-      <c r="H37" s="69"/>
-      <c r="I37" s="69"/>
-      <c r="J37" s="69"/>
-      <c r="K37" s="69"/>
-      <c r="L37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="70"/>
+      <c r="L37" s="71"/>
     </row>
     <row r="38" spans="1:15" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
@@ -10054,18 +10131,18 @@
       <c r="G39" s="40"/>
       <c r="H39" s="57">
         <f ca="1">Dice!C41*100</f>
-        <v>3000</v>
+        <v>2200</v>
       </c>
       <c r="I39" s="57">
         <f ca="1">Dice!C38*100</f>
-        <v>1700</v>
+        <v>1400</v>
       </c>
       <c r="J39" s="58" t="s">
         <v>414</v>
       </c>
-      <c r="K39" s="57">
-        <f ca="1">Dice!C37*10</f>
-        <v>110</v>
+      <c r="K39" s="57" t="e">
+        <f>Dice!#REF!*10</f>
+        <v>#REF!</v>
       </c>
       <c r="L39" s="59" t="s">
         <v>414</v>
@@ -10079,15 +10156,15 @@
         <v>425</v>
       </c>
       <c r="G40" s="41"/>
-      <c r="H40" s="73" t="s">
+      <c r="H40" s="74" t="s">
         <v>664</v>
       </c>
-      <c r="I40" s="73"/>
-      <c r="J40" s="71" t="s">
+      <c r="I40" s="74"/>
+      <c r="J40" s="72" t="s">
         <v>665</v>
       </c>
-      <c r="K40" s="71"/>
-      <c r="L40" s="72"/>
+      <c r="K40" s="72"/>
+      <c r="L40" s="73"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
@@ -10106,17 +10183,20 @@
         <f>(F41-E41)/100</f>
         <v>0.05</v>
       </c>
-      <c r="H41" s="74" t="s">
+      <c r="H41" s="67" t="s">
         <v>414</v>
       </c>
-      <c r="I41" s="74"/>
-      <c r="J41" s="74" t="s">
+      <c r="I41" s="67"/>
+      <c r="J41" s="67" t="s">
         <v>414</v>
       </c>
-      <c r="K41" s="74"/>
-      <c r="L41" s="75"/>
+      <c r="K41" s="67"/>
+      <c r="L41" s="68"/>
       <c r="M41" s="4" t="s">
         <v>667</v>
+      </c>
+      <c r="N41" s="83" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.15">
@@ -10136,16 +10216,19 @@
         <f t="shared" ref="G42:G56" si="4">(F42-E42)/100</f>
         <v>0.09</v>
       </c>
-      <c r="H42" s="67"/>
-      <c r="I42" s="67"/>
-      <c r="J42" s="74" t="s">
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="67" t="s">
         <v>414</v>
       </c>
-      <c r="K42" s="74"/>
-      <c r="L42" s="75"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="68"/>
       <c r="M42" s="4">
         <f ca="1">Dice!C37</f>
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="N42" s="4">
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.15">
@@ -10159,13 +10242,13 @@
         <f t="shared" si="4"/>
         <v>0.09</v>
       </c>
-      <c r="H43" s="67"/>
-      <c r="I43" s="67"/>
-      <c r="J43" s="74" t="s">
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="67" t="s">
         <v>414</v>
       </c>
-      <c r="K43" s="74"/>
-      <c r="L43" s="75"/>
+      <c r="K43" s="67"/>
+      <c r="L43" s="68"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="E44" s="4">
@@ -10178,13 +10261,13 @@
         <f t="shared" si="4"/>
         <v>0.09</v>
       </c>
-      <c r="H44" s="67"/>
-      <c r="I44" s="67"/>
-      <c r="J44" s="74" t="s">
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="67" t="s">
         <v>414</v>
       </c>
-      <c r="K44" s="74"/>
-      <c r="L44" s="75"/>
+      <c r="K44" s="67"/>
+      <c r="L44" s="68"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.15">
       <c r="E45" s="4">
@@ -10197,11 +10280,11 @@
         <f t="shared" si="4"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H45" s="67"/>
-      <c r="I45" s="67"/>
-      <c r="J45" s="67"/>
-      <c r="K45" s="67"/>
-      <c r="L45" s="77"/>
+      <c r="H45" s="63"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="63"/>
+      <c r="K45" s="63"/>
+      <c r="L45" s="64"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.15">
       <c r="E46" s="4">
@@ -10214,11 +10297,11 @@
         <f t="shared" si="4"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H46" s="67"/>
-      <c r="I46" s="67"/>
-      <c r="J46" s="67"/>
-      <c r="K46" s="67"/>
-      <c r="L46" s="77"/>
+      <c r="H46" s="63"/>
+      <c r="I46" s="63"/>
+      <c r="J46" s="63"/>
+      <c r="K46" s="63"/>
+      <c r="L46" s="64"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="E47" s="4">
@@ -10231,11 +10314,11 @@
         <f t="shared" si="4"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H47" s="67"/>
-      <c r="I47" s="67"/>
-      <c r="J47" s="67"/>
-      <c r="K47" s="67"/>
-      <c r="L47" s="77"/>
+      <c r="H47" s="63"/>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
+      <c r="K47" s="63"/>
+      <c r="L47" s="64"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.15">
       <c r="E48" s="4">
@@ -10248,11 +10331,11 @@
         <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
-      <c r="H48" s="67"/>
-      <c r="I48" s="67"/>
-      <c r="J48" s="67"/>
-      <c r="K48" s="67"/>
-      <c r="L48" s="77"/>
+      <c r="H48" s="63"/>
+      <c r="I48" s="63"/>
+      <c r="J48" s="63"/>
+      <c r="K48" s="63"/>
+      <c r="L48" s="64"/>
     </row>
     <row r="49" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E49" s="4">
@@ -10265,11 +10348,11 @@
         <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
-      <c r="H49" s="67"/>
-      <c r="I49" s="67"/>
-      <c r="J49" s="67"/>
-      <c r="K49" s="67"/>
-      <c r="L49" s="77"/>
+      <c r="H49" s="63"/>
+      <c r="I49" s="63"/>
+      <c r="J49" s="63"/>
+      <c r="K49" s="63"/>
+      <c r="L49" s="64"/>
     </row>
     <row r="50" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E50" s="4">
@@ -10282,11 +10365,11 @@
         <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
-      <c r="H50" s="67"/>
-      <c r="I50" s="67"/>
-      <c r="J50" s="67"/>
-      <c r="K50" s="67"/>
-      <c r="L50" s="77"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="63"/>
+      <c r="J50" s="63"/>
+      <c r="K50" s="63"/>
+      <c r="L50" s="64"/>
     </row>
     <row r="51" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E51" s="4">
@@ -10299,11 +10382,11 @@
         <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
-      <c r="H51" s="67"/>
-      <c r="I51" s="67"/>
-      <c r="J51" s="67"/>
-      <c r="K51" s="67"/>
-      <c r="L51" s="77"/>
+      <c r="H51" s="63"/>
+      <c r="I51" s="63"/>
+      <c r="J51" s="63"/>
+      <c r="K51" s="63"/>
+      <c r="L51" s="64"/>
     </row>
     <row r="52" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E52" s="4">
@@ -10316,11 +10399,11 @@
         <f t="shared" si="4"/>
         <v>0.01</v>
       </c>
-      <c r="H52" s="67"/>
-      <c r="I52" s="67"/>
-      <c r="J52" s="67"/>
-      <c r="K52" s="67"/>
-      <c r="L52" s="77"/>
+      <c r="H52" s="63"/>
+      <c r="I52" s="63"/>
+      <c r="J52" s="63"/>
+      <c r="K52" s="63"/>
+      <c r="L52" s="64"/>
     </row>
     <row r="53" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E53" s="4">
@@ -10333,11 +10416,11 @@
         <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
-      <c r="H53" s="67"/>
-      <c r="I53" s="67"/>
-      <c r="J53" s="67"/>
-      <c r="K53" s="67"/>
-      <c r="L53" s="77"/>
+      <c r="H53" s="63"/>
+      <c r="I53" s="63"/>
+      <c r="J53" s="63"/>
+      <c r="K53" s="63"/>
+      <c r="L53" s="64"/>
     </row>
     <row r="54" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E54" s="4">
@@ -10350,11 +10433,11 @@
         <f t="shared" si="4"/>
         <v>0.06</v>
       </c>
-      <c r="H54" s="67"/>
-      <c r="I54" s="67"/>
-      <c r="J54" s="67"/>
-      <c r="K54" s="67"/>
-      <c r="L54" s="77"/>
+      <c r="H54" s="63"/>
+      <c r="I54" s="63"/>
+      <c r="J54" s="63"/>
+      <c r="K54" s="63"/>
+      <c r="L54" s="64"/>
     </row>
     <row r="55" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E55" s="4">
@@ -10367,11 +10450,11 @@
         <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
-      <c r="H55" s="67"/>
-      <c r="I55" s="67"/>
-      <c r="J55" s="67"/>
-      <c r="K55" s="67"/>
-      <c r="L55" s="77"/>
+      <c r="H55" s="63"/>
+      <c r="I55" s="63"/>
+      <c r="J55" s="63"/>
+      <c r="K55" s="63"/>
+      <c r="L55" s="64"/>
     </row>
     <row r="56" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E56" s="4">
@@ -10384,11 +10467,11 @@
         <f t="shared" si="4"/>
         <v>0.01</v>
       </c>
-      <c r="H56" s="67"/>
-      <c r="I56" s="67"/>
-      <c r="J56" s="67"/>
-      <c r="K56" s="67"/>
-      <c r="L56" s="77"/>
+      <c r="H56" s="63"/>
+      <c r="I56" s="63"/>
+      <c r="J56" s="63"/>
+      <c r="K56" s="63"/>
+      <c r="L56" s="64"/>
     </row>
     <row r="57" spans="5:12" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="E57" s="34">
@@ -10401,28 +10484,27 @@
         <f>(F57-E57)/100</f>
         <v>9.8999999999999488E-3</v>
       </c>
-      <c r="H57" s="76"/>
-      <c r="I57" s="76"/>
-      <c r="J57" s="76"/>
-      <c r="K57" s="76"/>
-      <c r="L57" s="78"/>
+      <c r="H57" s="65"/>
+      <c r="I57" s="65"/>
+      <c r="J57" s="65"/>
+      <c r="K57" s="65"/>
+      <c r="L57" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="N18:T18"/>
-    <mergeCell ref="N2:U2"/>
-    <mergeCell ref="J54:L54"/>
-    <mergeCell ref="J55:L55"/>
-    <mergeCell ref="J56:L56"/>
-    <mergeCell ref="J57:L57"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="J48:L48"/>
-    <mergeCell ref="J49:L49"/>
-    <mergeCell ref="J50:L50"/>
-    <mergeCell ref="J51:L51"/>
-    <mergeCell ref="J52:L52"/>
-    <mergeCell ref="J53:L53"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="G37:L37"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
     <mergeCell ref="H55:I55"/>
     <mergeCell ref="H56:I56"/>
     <mergeCell ref="H57:I57"/>
@@ -10439,19 +10521,20 @@
     <mergeCell ref="H43:I43"/>
     <mergeCell ref="H44:I44"/>
     <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="G37:L37"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J57:L57"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="J48:L48"/>
+    <mergeCell ref="J49:L49"/>
+    <mergeCell ref="J50:L50"/>
+    <mergeCell ref="J51:L51"/>
+    <mergeCell ref="J52:L52"/>
+    <mergeCell ref="J53:L53"/>
+    <mergeCell ref="N18:T18"/>
+    <mergeCell ref="N2:U2"/>
+    <mergeCell ref="J54:L54"/>
+    <mergeCell ref="J55:L55"/>
+    <mergeCell ref="J56:L56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -10464,8 +10547,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:O100"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10532,7 +10615,7 @@
       </c>
       <c r="D3" s="23">
         <f ca="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" s="23">
         <f ca="1"/>
@@ -10540,11 +10623,11 @@
       </c>
       <c r="F3" s="23">
         <f ca="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" s="23">
         <f ca="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="23">
         <f ca="1"/>
@@ -10552,7 +10635,7 @@
       </c>
       <c r="I3" s="23">
         <f ca="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3" s="23">
         <f ca="1"/>
@@ -10564,7 +10647,7 @@
       </c>
       <c r="L3" s="23">
         <f ca="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.15">
@@ -10573,11 +10656,11 @@
       </c>
       <c r="C4" cm="1">
         <f t="array" aca="1" ref="C4:L4" ca="1">_xlfn.RANDARRAY(1,10,1,4, TRUE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <f ca="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <f ca="1"/>
@@ -10589,15 +10672,15 @@
       </c>
       <c r="G4">
         <f ca="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f ca="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I4">
         <f ca="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J4">
         <f ca="1"/>
@@ -10609,7 +10692,7 @@
       </c>
       <c r="L4">
         <f ca="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.15">
@@ -10622,19 +10705,19 @@
       </c>
       <c r="D5">
         <f ca="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <f ca="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <f ca="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <f ca="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <f ca="1"/>
@@ -10642,19 +10725,19 @@
       </c>
       <c r="I5">
         <f ca="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J5">
         <f ca="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K5">
         <f ca="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L5">
         <f ca="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
@@ -10667,39 +10750,39 @@
       </c>
       <c r="D6">
         <f ca="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <f ca="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6">
         <f ca="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6">
         <f ca="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H6">
         <f ca="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6">
         <f ca="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J6">
         <f ca="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K6">
         <f ca="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L6">
         <f ca="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.15">
@@ -10708,43 +10791,43 @@
       </c>
       <c r="C7" cm="1">
         <f t="array" aca="1" ref="C7:L7" ca="1">_xlfn.RANDARRAY(1,10,1,10, TRUE)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <f ca="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <f ca="1"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <f ca="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G7">
         <f ca="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H7">
         <f ca="1"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f ca="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J7">
         <f ca="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K7">
         <f ca="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L7">
         <f ca="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.15">
@@ -10753,19 +10836,19 @@
       </c>
       <c r="C8" cm="1">
         <f t="array" aca="1" ref="C8:L8" ca="1">_xlfn.RANDARRAY(1,10,1,12, TRUE)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <f ca="1"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <f ca="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <f ca="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G8">
         <f ca="1"/>
@@ -10773,23 +10856,23 @@
       </c>
       <c r="H8">
         <f ca="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <f ca="1"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J8">
         <f ca="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K8">
         <f ca="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L8">
         <f ca="1"/>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.15">
@@ -10802,39 +10885,39 @@
       </c>
       <c r="D9">
         <f ca="1"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E9">
         <f ca="1"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <f ca="1"/>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G9">
         <f ca="1"/>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H9">
         <f ca="1"/>
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="I9">
         <f ca="1"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J9">
         <f ca="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K9">
         <f ca="1"/>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="L9">
         <f ca="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.15">
@@ -10843,43 +10926,43 @@
       </c>
       <c r="C10" cm="1">
         <f t="array" aca="1" ref="C10:L10" ca="1">_xlfn.RANDARRAY(1,10,1,100, TRUE)</f>
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="D10">
         <f ca="1"/>
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E10">
         <f ca="1"/>
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="F10">
         <f ca="1"/>
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G10">
         <f ca="1"/>
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="H10">
         <f ca="1"/>
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="I10">
         <f ca="1"/>
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="J10">
         <f ca="1"/>
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="K10">
         <f ca="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L10">
         <f ca="1"/>
-        <v>86</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
@@ -10911,7 +10994,7 @@
       </c>
       <c r="C15">
         <f ca="1">SUM($C$3:$D$3)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="22" t="s">
@@ -10951,7 +11034,7 @@
       </c>
       <c r="C16">
         <f ca="1">SUM($C$3:$E$3)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>570</v>
@@ -10963,7 +11046,7 @@
       </c>
       <c r="C17">
         <f ca="1">SUM($C$3:$F$3)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>571</v>
@@ -10999,7 +11082,7 @@
       </c>
       <c r="C20">
         <f ca="1">SUM($C$3:$I$3)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>442</v>
@@ -11011,7 +11094,7 @@
       </c>
       <c r="C21">
         <f ca="1">SUM($C$3:$J$3)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.15">
@@ -11020,7 +11103,7 @@
       </c>
       <c r="C22">
         <f ca="1">SUM($C$3:$K$3)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E22" s="3"/>
     </row>
@@ -11030,7 +11113,7 @@
       </c>
       <c r="C23">
         <f ca="1">SUM(_xlfn.ANCHORARRAY($C$3))</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E23" s="3"/>
     </row>
@@ -11040,7 +11123,7 @@
       </c>
       <c r="C25">
         <f ca="1">SUM($C$4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.15">
@@ -11076,7 +11159,7 @@
       </c>
       <c r="C29">
         <f ca="1">SUM($C$4:$G$4)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.15">
@@ -11094,7 +11177,7 @@
       </c>
       <c r="C31">
         <f ca="1">SUM($C$4:$I$4)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.15">
@@ -11103,7 +11186,7 @@
       </c>
       <c r="C32">
         <f ca="1">SUM($C$4:$J$4)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.15">
@@ -11112,7 +11195,7 @@
       </c>
       <c r="C33">
         <f ca="1">SUM($C$4:$K$4)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.15">
@@ -11121,7 +11204,7 @@
       </c>
       <c r="C34">
         <f ca="1">SUM(_xlfn.ANCHORARRAY(C4))</f>
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.15">
@@ -11139,7 +11222,7 @@
       </c>
       <c r="C37">
         <f ca="1">SUM($C$5:$D$5)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.15">
@@ -11148,7 +11231,7 @@
       </c>
       <c r="C38">
         <f ca="1">SUM($C$5:$E$5)</f>
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.15">
@@ -11157,7 +11240,7 @@
       </c>
       <c r="C39">
         <f ca="1">SUM($C$5:$F$5)</f>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.15">
@@ -11166,7 +11249,7 @@
       </c>
       <c r="C40">
         <f ca="1">SUM($C$5:$G$5)</f>
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.15">
@@ -11175,7 +11258,7 @@
       </c>
       <c r="C41">
         <f ca="1">SUM($C$5:$H$5)</f>
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.15">
@@ -11184,7 +11267,7 @@
       </c>
       <c r="C42">
         <f ca="1">SUM($C$5:$I$5)</f>
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.15">
@@ -11193,7 +11276,7 @@
       </c>
       <c r="C43">
         <f ca="1">SUM($C$5:$J$5)</f>
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.15">
@@ -11202,7 +11285,7 @@
       </c>
       <c r="C44">
         <f ca="1">SUM($C$5:$K$5)</f>
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.15">
@@ -11211,7 +11294,7 @@
       </c>
       <c r="C45">
         <f ca="1">SUM(_xlfn.ANCHORARRAY(C5))</f>
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.15">
@@ -11229,7 +11312,7 @@
       </c>
       <c r="C48">
         <f ca="1">SUM(C6:D6)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.15">
@@ -11238,7 +11321,7 @@
       </c>
       <c r="C49">
         <f ca="1">SUM(C6:E6)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.15">
@@ -11247,7 +11330,7 @@
       </c>
       <c r="C50">
         <f ca="1">SUM(C6:F6)</f>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.15">
@@ -11256,7 +11339,7 @@
       </c>
       <c r="C51">
         <f ca="1">SUM(C6:G6)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.15">
@@ -11274,7 +11357,7 @@
       </c>
       <c r="C53">
         <f ca="1">SUM(C6:I6)</f>
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.15">
@@ -11283,7 +11366,7 @@
       </c>
       <c r="C54">
         <f ca="1">SUM(C6:J6)</f>
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.15">
@@ -11292,7 +11375,7 @@
       </c>
       <c r="C55">
         <f ca="1">SUM(C6:K6)</f>
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.15">
@@ -11301,7 +11384,7 @@
       </c>
       <c r="C56">
         <f ca="1">SUM(_xlfn.ANCHORARRAY(C6))</f>
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.15">
@@ -11310,7 +11393,7 @@
       </c>
       <c r="C58">
         <f ca="1">SUM(C7)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.15">
@@ -11319,7 +11402,7 @@
       </c>
       <c r="C59">
         <f ca="1">SUM(C7:D7)</f>
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.15">
@@ -11328,7 +11411,7 @@
       </c>
       <c r="C60">
         <f ca="1">SUM(C7:E7)</f>
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.15">
@@ -11337,7 +11420,7 @@
       </c>
       <c r="C61">
         <f ca="1">SUM(C7:F7)</f>
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.15">
@@ -11346,7 +11429,7 @@
       </c>
       <c r="C62">
         <f ca="1">SUM(C7:G7)</f>
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.15">
@@ -11355,7 +11438,7 @@
       </c>
       <c r="C63">
         <f ca="1">SUM(C7:H7)</f>
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.15">
@@ -11364,7 +11447,7 @@
       </c>
       <c r="C64">
         <f ca="1">SUM(C7:I7)</f>
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.15">
@@ -11373,7 +11456,7 @@
       </c>
       <c r="C65">
         <f ca="1">SUM(C7:J7)</f>
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.15">
@@ -11382,7 +11465,7 @@
       </c>
       <c r="C66" s="4">
         <f ca="1">SUM(C7:K7)</f>
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.15">
@@ -11391,7 +11474,7 @@
       </c>
       <c r="C67">
         <f ca="1">SUM(_xlfn.ANCHORARRAY(C7))</f>
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.15">
@@ -11400,7 +11483,7 @@
       </c>
       <c r="C69">
         <f ca="1">SUM(C8)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.15">
@@ -11409,7 +11492,7 @@
       </c>
       <c r="C70">
         <f ca="1">SUM(C8:D8)</f>
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.15">
@@ -11418,7 +11501,7 @@
       </c>
       <c r="C71">
         <f ca="1">SUM(C8:E8)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.15">
@@ -11445,7 +11528,7 @@
       </c>
       <c r="C74">
         <f ca="1">SUM(C8:H8)</f>
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.15">
@@ -11454,7 +11537,7 @@
       </c>
       <c r="C75">
         <f ca="1">SUM(C8:I8)</f>
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.15">
@@ -11463,7 +11546,7 @@
       </c>
       <c r="C76">
         <f ca="1">SUM(C8:J8)</f>
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.15">
@@ -11472,7 +11555,7 @@
       </c>
       <c r="C77">
         <f ca="1">SUM(C8:K8)</f>
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.15">
@@ -11481,7 +11564,7 @@
       </c>
       <c r="C78">
         <f ca="1">SUM(_xlfn.ANCHORARRAY(C8))</f>
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.15">
@@ -11499,7 +11582,7 @@
       </c>
       <c r="C81">
         <f ca="1">SUM(C9:D9)</f>
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.15">
@@ -11508,7 +11591,7 @@
       </c>
       <c r="C82">
         <f ca="1">SUM(C9:E9)</f>
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.15">
@@ -11517,7 +11600,7 @@
       </c>
       <c r="C83">
         <f ca="1">SUM(C9:F9)</f>
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.15">
@@ -11526,7 +11609,7 @@
       </c>
       <c r="C84">
         <f ca="1">SUM(C9:G9)</f>
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.15">
@@ -11535,7 +11618,7 @@
       </c>
       <c r="C85">
         <f ca="1">SUM(C9:H9)</f>
-        <v>65</v>
+        <v>89</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.15">
@@ -11544,7 +11627,7 @@
       </c>
       <c r="C86">
         <f ca="1">SUM(C9:I9)</f>
-        <v>68</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.15">
@@ -11553,7 +11636,7 @@
       </c>
       <c r="C87">
         <f ca="1">SUM(C9:J9)</f>
-        <v>88</v>
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.15">
@@ -11562,7 +11645,7 @@
       </c>
       <c r="C88">
         <f ca="1">SUM(C9:K9)</f>
-        <v>89</v>
+        <v>130</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.15">
@@ -11571,7 +11654,7 @@
       </c>
       <c r="C89">
         <f ca="1">SUM(_xlfn.ANCHORARRAY(C9))</f>
-        <v>93</v>
+        <v>132</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.15">
@@ -11580,7 +11663,7 @@
       </c>
       <c r="C91">
         <f ca="1">SUM(C10)</f>
-        <v>42</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.15">
@@ -11589,7 +11672,7 @@
       </c>
       <c r="C92">
         <f ca="1">SUM(C10:D10)</f>
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.15">
@@ -11598,7 +11681,7 @@
       </c>
       <c r="C93">
         <f ca="1">SUM(C10:E10)</f>
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.15">
@@ -11607,7 +11690,7 @@
       </c>
       <c r="C94">
         <f ca="1">SUM(C10:F10)</f>
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.15">
@@ -11616,7 +11699,7 @@
       </c>
       <c r="C95">
         <f ca="1">SUM(C10:G10)</f>
-        <v>231</v>
+        <v>251</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.15">
@@ -11625,7 +11708,7 @@
       </c>
       <c r="C96">
         <f ca="1">SUM(C10:H10)</f>
-        <v>285</v>
+        <v>266</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.15">
@@ -11634,7 +11717,7 @@
       </c>
       <c r="C97">
         <f ca="1">SUM(C10:I10)</f>
-        <v>377</v>
+        <v>365</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.15">
@@ -11643,7 +11726,7 @@
       </c>
       <c r="C98">
         <f ca="1">SUM(C10:J10)</f>
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.15">
@@ -11652,7 +11735,7 @@
       </c>
       <c r="C99">
         <f ca="1">SUM(C10:K10)</f>
-        <v>433</v>
+        <v>438</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.15">
@@ -11661,7 +11744,7 @@
       </c>
       <c r="C100">
         <f ca="1">SUM(_xlfn.ANCHORARRAY(C10))</f>
-        <v>519</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -11904,18 +11987,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11938,14 +12021,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5630E48F-06FF-40E7-BF4D-59B62F08489A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C7B6BB1-D811-49AB-9F03-CED9DA2029E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -11960,4 +12035,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5630E48F-06FF-40E7-BF4D-59B62F08489A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>